<commit_message>
fix formats for employee importer
</commit_message>
<xml_diff>
--- a/src/assets/formats/update-employee-status.xlsx
+++ b/src/assets/formats/update-employee-status.xlsx
@@ -74,7 +74,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -97,11 +97,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -114,6 +127,9 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -384,7 +400,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -395,7 +411,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -419,16 +435,16 @@
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="1" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>